<commit_message>
Added Rules and words
</commit_message>
<xml_diff>
--- a/Adjectives.xlsx
+++ b/Adjectives.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880F934F-305E-4B5E-A22A-1EB57C44147F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C330C99-6124-454B-B2CB-EC4F63181C69}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Colors" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="704">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="705">
   <si>
     <t>Alizarin</t>
   </si>
@@ -2136,6 +2136,9 @@
   </si>
   <si>
     <t>wedge</t>
+  </si>
+  <si>
+    <t>bijou</t>
   </si>
 </sst>
 </file>
@@ -3045,8 +3048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA78D6B7-4323-4276-8102-EF5BBEC08473}">
   <dimension ref="A1:Y22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3451,7 +3454,9 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>704</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -5150,8 +5155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E4367A-CBFB-4099-BC2B-F12E88C4A933}">
   <dimension ref="A1:W12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
It makes passwords based off of rules
Next is the sentence!
</commit_message>
<xml_diff>
--- a/Adjectives.xlsx
+++ b/Adjectives.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C330C99-6124-454B-B2CB-EC4F63181C69}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59EE18E-5F36-4919-9584-176194E6C3F5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Colors" sheetId="1" r:id="rId1"/>
@@ -3048,7 +3048,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA78D6B7-4323-4276-8102-EF5BBEC08473}">
   <dimension ref="A1:Y22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -5155,13 +5155,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E4367A-CBFB-4099-BC2B-F12E88C4A933}">
   <dimension ref="A1:W12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8:E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>